<commit_message>
Planung des 4. Sprints
</commit_message>
<xml_diff>
--- a/Projektleiter/GanttChart_4_Semester.xlsx
+++ b/Projektleiter/GanttChart_4_Semester.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D79EF0-767D-41E0-90A6-B2028C1552CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DDA86F-F09F-4537-AF0D-3C909F49152B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -130,12 +130,6 @@
     <t>Modelling Wizard - TINF19C</t>
   </si>
   <si>
-    <t>Woche 1 Sprint</t>
-  </si>
-  <si>
-    <t>Woche 2 Sprint</t>
-  </si>
-  <si>
     <t>Firmenname : DHBW-Gruppe 2</t>
   </si>
   <si>
@@ -160,15 +154,9 @@
     <t>Aufsetzen der Entwicklungsumgebung des Teams</t>
   </si>
   <si>
-    <t>Non-Functional Requirements im Backlog</t>
-  </si>
-  <si>
     <t>SJ, TR, PT</t>
   </si>
   <si>
-    <t>Functional Requirement im Backlog</t>
-  </si>
-  <si>
     <t>PT, JS, TZ</t>
   </si>
   <si>
@@ -182,6 +170,99 @@
   </si>
   <si>
     <t>SB,TZ, TR, SJ, PT, JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raj Kumar Pulaparthi - Meeting </t>
+  </si>
+  <si>
+    <t>Non-Functional: NF10,NF30,NF50, NF70</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS Anpassung </t>
+  </si>
+  <si>
+    <t>TR,TZ</t>
+  </si>
+  <si>
+    <t>2 Sprint</t>
+  </si>
+  <si>
+    <t>1 Sprint</t>
+  </si>
+  <si>
+    <t>3 Sprint</t>
+  </si>
+  <si>
+    <t>Non-Functional: NF20</t>
+  </si>
+  <si>
+    <t>Functional: F10, F20, F70</t>
+  </si>
+  <si>
+    <t>Allgemeiner Test</t>
+  </si>
+  <si>
+    <t>Non-Functional: NF40, NF60, NF80, NF90, NF100</t>
+  </si>
+  <si>
+    <t>4 Sprint</t>
+  </si>
+  <si>
+    <t>Non-Functional: NF100</t>
+  </si>
+  <si>
+    <t>Functional:  F50, F80</t>
+  </si>
+  <si>
+    <t>Functional: F30, F60, F40</t>
+  </si>
+  <si>
+    <t>Projekt für Kundenpräsentation fertigstellen</t>
+  </si>
+  <si>
+    <t>SJ,SB</t>
+  </si>
+  <si>
+    <t>Modulhandbuch</t>
+  </si>
+  <si>
+    <t>Usermanual</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>System Test Plan</t>
+  </si>
+  <si>
+    <t>System Test Report</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Business Case, Projekthandbuch</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Selbstkritik, Lessons Learned</t>
+  </si>
+  <si>
+    <t>Anpassung des SRS und CRS</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>Anpassung des SAS</t>
+  </si>
+  <si>
+    <t>SJ</t>
   </si>
 </sst>
 </file>
@@ -195,10 +276,10 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="d\.m\.yy;@"/>
-    <numFmt numFmtId="169" formatCode="d"/>
-    <numFmt numFmtId="170" formatCode="d/\ mmm\ yyyy"/>
-    <numFmt numFmtId="171" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="173" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="d"/>
+    <numFmt numFmtId="169" formatCode="d/\ mmm\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="171" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -875,7 +956,7 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="2" applyFill="0">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyFill="0">
@@ -1035,13 +1116,13 @@
     <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,44 +1152,44 @@
     <xf numFmtId="167" fontId="9" fillId="41" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="40" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="42" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="42" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="40" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="42" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="42" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1661,11 +1742,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL25"/>
+  <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:C4"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I2" s="27"/>
     </row>
@@ -1710,110 +1791,110 @@
         <v>2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="65">
         <v>44263</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="65"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="57"/>
+      <c r="B4" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="64"/>
       <c r="D4" s="46" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="54">
+      <c r="I4" s="61">
         <f>I5</f>
         <v>44263</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="54">
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="61">
         <f>P5</f>
         <v>44270</v>
       </c>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="54">
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="61">
         <f>W5</f>
         <v>44277</v>
       </c>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="56"/>
-      <c r="AD4" s="54">
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="61">
         <f>AD5</f>
         <v>44284</v>
       </c>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="55"/>
-      <c r="AG4" s="55"/>
-      <c r="AH4" s="55"/>
-      <c r="AI4" s="55"/>
-      <c r="AJ4" s="56"/>
-      <c r="AK4" s="54">
+      <c r="AE4" s="62"/>
+      <c r="AF4" s="62"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="62"/>
+      <c r="AI4" s="62"/>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="61">
         <f>AK5</f>
         <v>44291</v>
       </c>
-      <c r="AL4" s="55"/>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="55"/>
-      <c r="AO4" s="55"/>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="56"/>
-      <c r="AR4" s="54">
+      <c r="AL4" s="62"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="62"/>
+      <c r="AO4" s="62"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="63"/>
+      <c r="AR4" s="61">
         <f>AR5</f>
         <v>44298</v>
       </c>
-      <c r="AS4" s="55"/>
-      <c r="AT4" s="55"/>
-      <c r="AU4" s="55"/>
-      <c r="AV4" s="55"/>
-      <c r="AW4" s="55"/>
-      <c r="AX4" s="56"/>
-      <c r="AY4" s="54">
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="63"/>
+      <c r="AY4" s="61">
         <f>AY5</f>
         <v>44305</v>
       </c>
-      <c r="AZ4" s="55"/>
-      <c r="BA4" s="55"/>
-      <c r="BB4" s="55"/>
-      <c r="BC4" s="55"/>
-      <c r="BD4" s="55"/>
-      <c r="BE4" s="56"/>
-      <c r="BF4" s="54">
+      <c r="AZ4" s="62"/>
+      <c r="BA4" s="62"/>
+      <c r="BB4" s="62"/>
+      <c r="BC4" s="62"/>
+      <c r="BD4" s="62"/>
+      <c r="BE4" s="63"/>
+      <c r="BF4" s="61">
         <f>BF5</f>
         <v>44312</v>
       </c>
-      <c r="BG4" s="55"/>
-      <c r="BH4" s="55"/>
-      <c r="BI4" s="55"/>
-      <c r="BJ4" s="55"/>
-      <c r="BK4" s="55"/>
-      <c r="BL4" s="56"/>
+      <c r="BG4" s="62"/>
+      <c r="BH4" s="62"/>
+      <c r="BI4" s="62"/>
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="63"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
@@ -2370,7 +2451,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="15"/>
@@ -2378,7 +2459,7 @@
       <c r="F8" s="36"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H22" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H36" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="43"/>
@@ -2443,10 +2524,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -2523,10 +2604,10 @@
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2600,10 +2681,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="16">
         <v>1</v>
@@ -2676,13 +2757,13 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="34" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="16">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="37">
         <v>44270</v>
@@ -2752,13 +2833,13 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="34" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13" s="16">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E13" s="37">
         <v>44270</v>
@@ -2828,13 +2909,13 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
       <c r="B14" s="34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="37">
         <v>44279</v>
@@ -2903,20 +2984,20 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="65">
-        <v>0</v>
-      </c>
-      <c r="E15" s="66">
-        <v>44281</v>
-      </c>
-      <c r="F15" s="66">
-        <v>44281</v>
+      <c r="C15" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="37">
+        <v>44280</v>
+      </c>
+      <c r="F15" s="37">
+        <v>44280</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -2979,13 +3060,21 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
-      <c r="B16" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="B16" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="59">
+        <v>1</v>
+      </c>
+      <c r="E16" s="60">
+        <v>44281</v>
+      </c>
+      <c r="F16" s="60">
+        <v>44281</v>
+      </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="43"/>
@@ -3047,21 +3136,13 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25"/>
-      <c r="B17" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="52">
-        <v>0</v>
-      </c>
-      <c r="E17" s="53">
-        <v>44281</v>
-      </c>
-      <c r="F17" s="53">
-        <v>44289</v>
-      </c>
+      <c r="B17" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="43"/>
@@ -3124,13 +3205,13 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
       <c r="B18" s="50" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="59">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="D18" s="52">
+        <v>1</v>
       </c>
       <c r="E18" s="53">
         <v>44281</v>
@@ -3199,11 +3280,21 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
+      <c r="B19" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="54">
+        <v>1</v>
+      </c>
+      <c r="E19" s="53">
+        <v>44281</v>
+      </c>
+      <c r="F19" s="53">
+        <v>44289</v>
+      </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="43"/>
@@ -3265,11 +3356,21 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="B20" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="54">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="53">
+        <v>44281</v>
+      </c>
+      <c r="F20" s="53">
+        <v>44302</v>
+      </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="43"/>
@@ -3330,19 +3431,16 @@
       <c r="BL20" s="21"/>
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H21" s="13"/>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
       <c r="K21" s="43"/>
@@ -3355,8 +3453,8 @@
       <c r="R21" s="43"/>
       <c r="S21" s="43"/>
       <c r="T21" s="43"/>
-      <c r="U21" s="44"/>
-      <c r="V21" s="44"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
       <c r="W21" s="43"/>
       <c r="X21" s="43"/>
       <c r="Y21" s="43"/>
@@ -3401,87 +3499,1148 @@
       <c r="BL21" s="21"/>
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="52">
+        <v>0</v>
+      </c>
+      <c r="E22" s="53">
+        <v>44291</v>
+      </c>
+      <c r="F22" s="53">
+        <v>44302</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="43"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="43"/>
+      <c r="AL22" s="43"/>
+      <c r="AM22" s="43"/>
+      <c r="AN22" s="43"/>
+      <c r="AO22" s="43"/>
+      <c r="AP22" s="43"/>
+      <c r="AQ22" s="43"/>
+      <c r="AR22" s="43"/>
+      <c r="AS22" s="43"/>
+      <c r="AT22" s="43"/>
+      <c r="AU22" s="43"/>
+      <c r="AV22" s="43"/>
+      <c r="AW22" s="43"/>
+      <c r="AX22" s="43"/>
+      <c r="AY22" s="43"/>
+      <c r="AZ22" s="43"/>
+      <c r="BA22" s="43"/>
+      <c r="BB22" s="43"/>
+      <c r="BC22" s="43"/>
+      <c r="BD22" s="43"/>
+      <c r="BE22" s="43"/>
+      <c r="BF22" s="43"/>
+      <c r="BG22" s="43"/>
+      <c r="BH22" s="43"/>
+      <c r="BI22" s="43"/>
+      <c r="BJ22" s="21"/>
+      <c r="BK22" s="21"/>
+      <c r="BL22" s="21"/>
+    </row>
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="54">
+        <v>0</v>
+      </c>
+      <c r="E23" s="53">
+        <v>44291</v>
+      </c>
+      <c r="F23" s="53">
+        <v>44302</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="43"/>
+      <c r="AC23" s="43"/>
+      <c r="AD23" s="43"/>
+      <c r="AE23" s="43"/>
+      <c r="AF23" s="43"/>
+      <c r="AG23" s="43"/>
+      <c r="AH23" s="43"/>
+      <c r="AI23" s="43"/>
+      <c r="AJ23" s="43"/>
+      <c r="AK23" s="43"/>
+      <c r="AL23" s="43"/>
+      <c r="AM23" s="43"/>
+      <c r="AN23" s="43"/>
+      <c r="AO23" s="43"/>
+      <c r="AP23" s="43"/>
+      <c r="AQ23" s="43"/>
+      <c r="AR23" s="43"/>
+      <c r="AS23" s="43"/>
+      <c r="AT23" s="43"/>
+      <c r="AU23" s="43"/>
+      <c r="AV23" s="43"/>
+      <c r="AW23" s="43"/>
+      <c r="AX23" s="43"/>
+      <c r="AY23" s="43"/>
+      <c r="AZ23" s="43"/>
+      <c r="BA23" s="43"/>
+      <c r="BB23" s="43"/>
+      <c r="BC23" s="43"/>
+      <c r="BD23" s="43"/>
+      <c r="BE23" s="43"/>
+      <c r="BF23" s="43"/>
+      <c r="BG23" s="43"/>
+      <c r="BH23" s="43"/>
+      <c r="BI23" s="43"/>
+      <c r="BJ23" s="21"/>
+      <c r="BK23" s="21"/>
+      <c r="BL23" s="21"/>
+    </row>
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="54">
+        <v>0</v>
+      </c>
+      <c r="E24" s="53">
+        <v>44291</v>
+      </c>
+      <c r="F24" s="53">
+        <v>44302</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="43"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="43"/>
+      <c r="AA24" s="43"/>
+      <c r="AB24" s="43"/>
+      <c r="AC24" s="43"/>
+      <c r="AD24" s="43"/>
+      <c r="AE24" s="43"/>
+      <c r="AF24" s="43"/>
+      <c r="AG24" s="43"/>
+      <c r="AH24" s="43"/>
+      <c r="AI24" s="43"/>
+      <c r="AJ24" s="43"/>
+      <c r="AK24" s="43"/>
+      <c r="AL24" s="43"/>
+      <c r="AM24" s="43"/>
+      <c r="AN24" s="43"/>
+      <c r="AO24" s="43"/>
+      <c r="AP24" s="43"/>
+      <c r="AQ24" s="43"/>
+      <c r="AR24" s="43"/>
+      <c r="AS24" s="43"/>
+      <c r="AT24" s="43"/>
+      <c r="AU24" s="43"/>
+      <c r="AV24" s="43"/>
+      <c r="AW24" s="43"/>
+      <c r="AX24" s="43"/>
+      <c r="AY24" s="43"/>
+      <c r="AZ24" s="43"/>
+      <c r="BA24" s="43"/>
+      <c r="BB24" s="43"/>
+      <c r="BC24" s="43"/>
+      <c r="BD24" s="43"/>
+      <c r="BE24" s="43"/>
+      <c r="BF24" s="43"/>
+      <c r="BG24" s="43"/>
+      <c r="BH24" s="43"/>
+      <c r="BI24" s="43"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="21"/>
+      <c r="BL24" s="21"/>
+    </row>
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25"/>
+      <c r="B25" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="43"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="43"/>
+      <c r="AB25" s="43"/>
+      <c r="AC25" s="43"/>
+      <c r="AD25" s="43"/>
+      <c r="AE25" s="43"/>
+      <c r="AF25" s="43"/>
+      <c r="AG25" s="43"/>
+      <c r="AH25" s="43"/>
+      <c r="AI25" s="43"/>
+      <c r="AJ25" s="43"/>
+      <c r="AK25" s="43"/>
+      <c r="AL25" s="43"/>
+      <c r="AM25" s="43"/>
+      <c r="AN25" s="43"/>
+      <c r="AO25" s="43"/>
+      <c r="AP25" s="43"/>
+      <c r="AQ25" s="43"/>
+      <c r="AR25" s="43"/>
+      <c r="AS25" s="43"/>
+      <c r="AT25" s="43"/>
+      <c r="AU25" s="43"/>
+      <c r="AV25" s="43"/>
+      <c r="AW25" s="43"/>
+      <c r="AX25" s="43"/>
+      <c r="AY25" s="43"/>
+      <c r="AZ25" s="43"/>
+      <c r="BA25" s="43"/>
+      <c r="BB25" s="43"/>
+      <c r="BC25" s="43"/>
+      <c r="BD25" s="43"/>
+      <c r="BE25" s="43"/>
+      <c r="BF25" s="43"/>
+      <c r="BG25" s="43"/>
+      <c r="BH25" s="43"/>
+      <c r="BI25" s="43"/>
+      <c r="BJ25" s="21"/>
+      <c r="BK25" s="21"/>
+      <c r="BL25" s="21"/>
+    </row>
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="52">
+        <v>0</v>
+      </c>
+      <c r="E26" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F26" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="43"/>
+      <c r="AA26" s="43"/>
+      <c r="AB26" s="43"/>
+      <c r="AC26" s="43"/>
+      <c r="AD26" s="43"/>
+      <c r="AE26" s="43"/>
+      <c r="AF26" s="43"/>
+      <c r="AG26" s="43"/>
+      <c r="AH26" s="43"/>
+      <c r="AI26" s="43"/>
+      <c r="AJ26" s="43"/>
+      <c r="AK26" s="43"/>
+      <c r="AL26" s="43"/>
+      <c r="AM26" s="43"/>
+      <c r="AN26" s="43"/>
+      <c r="AO26" s="43"/>
+      <c r="AP26" s="43"/>
+      <c r="AQ26" s="43"/>
+      <c r="AR26" s="43"/>
+      <c r="AS26" s="43"/>
+      <c r="AT26" s="43"/>
+      <c r="AU26" s="43"/>
+      <c r="AV26" s="43"/>
+      <c r="AW26" s="43"/>
+      <c r="AX26" s="43"/>
+      <c r="AY26" s="43"/>
+      <c r="AZ26" s="43"/>
+      <c r="BA26" s="43"/>
+      <c r="BB26" s="43"/>
+      <c r="BC26" s="43"/>
+      <c r="BD26" s="43"/>
+      <c r="BE26" s="43"/>
+      <c r="BF26" s="43"/>
+      <c r="BG26" s="43"/>
+      <c r="BH26" s="43"/>
+      <c r="BI26" s="43"/>
+      <c r="BJ26" s="21"/>
+      <c r="BK26" s="21"/>
+      <c r="BL26" s="21"/>
+    </row>
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25"/>
+      <c r="B27" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="52">
+        <v>0</v>
+      </c>
+      <c r="E27" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F27" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="43"/>
+      <c r="Z27" s="43"/>
+      <c r="AA27" s="43"/>
+      <c r="AB27" s="43"/>
+      <c r="AC27" s="43"/>
+      <c r="AD27" s="43"/>
+      <c r="AE27" s="43"/>
+      <c r="AF27" s="43"/>
+      <c r="AG27" s="43"/>
+      <c r="AH27" s="43"/>
+      <c r="AI27" s="43"/>
+      <c r="AJ27" s="43"/>
+      <c r="AK27" s="43"/>
+      <c r="AL27" s="43"/>
+      <c r="AM27" s="43"/>
+      <c r="AN27" s="43"/>
+      <c r="AO27" s="43"/>
+      <c r="AP27" s="43"/>
+      <c r="AQ27" s="43"/>
+      <c r="AR27" s="43"/>
+      <c r="AS27" s="43"/>
+      <c r="AT27" s="43"/>
+      <c r="AU27" s="43"/>
+      <c r="AV27" s="43"/>
+      <c r="AW27" s="43"/>
+      <c r="AX27" s="43"/>
+      <c r="AY27" s="43"/>
+      <c r="AZ27" s="43"/>
+      <c r="BA27" s="43"/>
+      <c r="BB27" s="43"/>
+      <c r="BC27" s="43"/>
+      <c r="BD27" s="43"/>
+      <c r="BE27" s="43"/>
+      <c r="BF27" s="43"/>
+      <c r="BG27" s="43"/>
+      <c r="BH27" s="43"/>
+      <c r="BI27" s="43"/>
+      <c r="BJ27" s="21"/>
+      <c r="BK27" s="21"/>
+      <c r="BL27" s="21"/>
+    </row>
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
+      <c r="B28" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="52">
+        <v>0</v>
+      </c>
+      <c r="E28" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F28" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
+      <c r="W28" s="43"/>
+      <c r="X28" s="43"/>
+      <c r="Y28" s="43"/>
+      <c r="Z28" s="43"/>
+      <c r="AA28" s="43"/>
+      <c r="AB28" s="43"/>
+      <c r="AC28" s="43"/>
+      <c r="AD28" s="43"/>
+      <c r="AE28" s="43"/>
+      <c r="AF28" s="43"/>
+      <c r="AG28" s="43"/>
+      <c r="AH28" s="43"/>
+      <c r="AI28" s="43"/>
+      <c r="AJ28" s="43"/>
+      <c r="AK28" s="43"/>
+      <c r="AL28" s="43"/>
+      <c r="AM28" s="43"/>
+      <c r="AN28" s="43"/>
+      <c r="AO28" s="43"/>
+      <c r="AP28" s="43"/>
+      <c r="AQ28" s="43"/>
+      <c r="AR28" s="43"/>
+      <c r="AS28" s="43"/>
+      <c r="AT28" s="43"/>
+      <c r="AU28" s="43"/>
+      <c r="AV28" s="43"/>
+      <c r="AW28" s="43"/>
+      <c r="AX28" s="43"/>
+      <c r="AY28" s="43"/>
+      <c r="AZ28" s="43"/>
+      <c r="BA28" s="43"/>
+      <c r="BB28" s="43"/>
+      <c r="BC28" s="43"/>
+      <c r="BD28" s="43"/>
+      <c r="BE28" s="43"/>
+      <c r="BF28" s="43"/>
+      <c r="BG28" s="43"/>
+      <c r="BH28" s="43"/>
+      <c r="BI28" s="43"/>
+      <c r="BJ28" s="21"/>
+      <c r="BK28" s="21"/>
+      <c r="BL28" s="21"/>
+    </row>
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25"/>
+      <c r="B29" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="52">
+        <v>0</v>
+      </c>
+      <c r="E29" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F29" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G29" s="66"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+      <c r="T29" s="43"/>
+      <c r="U29" s="43"/>
+      <c r="V29" s="43"/>
+      <c r="W29" s="43"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="43"/>
+      <c r="Z29" s="43"/>
+      <c r="AA29" s="43"/>
+      <c r="AB29" s="43"/>
+      <c r="AC29" s="43"/>
+      <c r="AD29" s="43"/>
+      <c r="AE29" s="43"/>
+      <c r="AF29" s="43"/>
+      <c r="AG29" s="43"/>
+      <c r="AH29" s="43"/>
+      <c r="AI29" s="43"/>
+      <c r="AJ29" s="43"/>
+      <c r="AK29" s="43"/>
+      <c r="AL29" s="43"/>
+      <c r="AM29" s="43"/>
+      <c r="AN29" s="43"/>
+      <c r="AO29" s="43"/>
+      <c r="AP29" s="43"/>
+      <c r="AQ29" s="43"/>
+      <c r="AR29" s="43"/>
+      <c r="AS29" s="43"/>
+      <c r="AT29" s="43"/>
+      <c r="AU29" s="43"/>
+      <c r="AV29" s="43"/>
+      <c r="AW29" s="43"/>
+      <c r="AX29" s="43"/>
+      <c r="AY29" s="43"/>
+      <c r="AZ29" s="43"/>
+      <c r="BA29" s="43"/>
+      <c r="BB29" s="43"/>
+      <c r="BC29" s="43"/>
+      <c r="BD29" s="43"/>
+      <c r="BE29" s="43"/>
+      <c r="BF29" s="43"/>
+      <c r="BG29" s="43"/>
+      <c r="BH29" s="43"/>
+      <c r="BI29" s="43"/>
+      <c r="BJ29" s="21"/>
+      <c r="BK29" s="21"/>
+      <c r="BL29" s="21"/>
+    </row>
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
+      <c r="B30" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="52">
+        <v>0</v>
+      </c>
+      <c r="E30" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F30" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G30" s="66"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+      <c r="U30" s="43"/>
+      <c r="V30" s="43"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="43"/>
+      <c r="Y30" s="43"/>
+      <c r="Z30" s="43"/>
+      <c r="AA30" s="43"/>
+      <c r="AB30" s="43"/>
+      <c r="AC30" s="43"/>
+      <c r="AD30" s="43"/>
+      <c r="AE30" s="43"/>
+      <c r="AF30" s="43"/>
+      <c r="AG30" s="43"/>
+      <c r="AH30" s="43"/>
+      <c r="AI30" s="43"/>
+      <c r="AJ30" s="43"/>
+      <c r="AK30" s="43"/>
+      <c r="AL30" s="43"/>
+      <c r="AM30" s="43"/>
+      <c r="AN30" s="43"/>
+      <c r="AO30" s="43"/>
+      <c r="AP30" s="43"/>
+      <c r="AQ30" s="43"/>
+      <c r="AR30" s="43"/>
+      <c r="AS30" s="43"/>
+      <c r="AT30" s="43"/>
+      <c r="AU30" s="43"/>
+      <c r="AV30" s="43"/>
+      <c r="AW30" s="43"/>
+      <c r="AX30" s="43"/>
+      <c r="AY30" s="43"/>
+      <c r="AZ30" s="43"/>
+      <c r="BA30" s="43"/>
+      <c r="BB30" s="43"/>
+      <c r="BC30" s="43"/>
+      <c r="BD30" s="43"/>
+      <c r="BE30" s="43"/>
+      <c r="BF30" s="43"/>
+      <c r="BG30" s="43"/>
+      <c r="BH30" s="43"/>
+      <c r="BI30" s="43"/>
+      <c r="BJ30" s="21"/>
+      <c r="BK30" s="21"/>
+      <c r="BL30" s="21"/>
+    </row>
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
+      <c r="B31" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="52">
+        <v>0</v>
+      </c>
+      <c r="E31" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F31" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G31" s="66"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+      <c r="U31" s="43"/>
+      <c r="V31" s="43"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="43"/>
+      <c r="Y31" s="43"/>
+      <c r="Z31" s="43"/>
+      <c r="AA31" s="43"/>
+      <c r="AB31" s="43"/>
+      <c r="AC31" s="43"/>
+      <c r="AD31" s="43"/>
+      <c r="AE31" s="43"/>
+      <c r="AF31" s="43"/>
+      <c r="AG31" s="43"/>
+      <c r="AH31" s="43"/>
+      <c r="AI31" s="43"/>
+      <c r="AJ31" s="43"/>
+      <c r="AK31" s="43"/>
+      <c r="AL31" s="43"/>
+      <c r="AM31" s="43"/>
+      <c r="AN31" s="43"/>
+      <c r="AO31" s="43"/>
+      <c r="AP31" s="43"/>
+      <c r="AQ31" s="43"/>
+      <c r="AR31" s="43"/>
+      <c r="AS31" s="43"/>
+      <c r="AT31" s="43"/>
+      <c r="AU31" s="43"/>
+      <c r="AV31" s="43"/>
+      <c r="AW31" s="43"/>
+      <c r="AX31" s="43"/>
+      <c r="AY31" s="43"/>
+      <c r="AZ31" s="43"/>
+      <c r="BA31" s="43"/>
+      <c r="BB31" s="43"/>
+      <c r="BC31" s="43"/>
+      <c r="BD31" s="43"/>
+      <c r="BE31" s="43"/>
+      <c r="BF31" s="43"/>
+      <c r="BG31" s="43"/>
+      <c r="BH31" s="43"/>
+      <c r="BI31" s="43"/>
+      <c r="BJ31" s="21"/>
+      <c r="BK31" s="21"/>
+      <c r="BL31" s="21"/>
+    </row>
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
+      <c r="B32" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="52">
+        <v>0</v>
+      </c>
+      <c r="E32" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F32" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G32" s="66"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
+      <c r="Z32" s="43"/>
+      <c r="AA32" s="43"/>
+      <c r="AB32" s="43"/>
+      <c r="AC32" s="43"/>
+      <c r="AD32" s="43"/>
+      <c r="AE32" s="43"/>
+      <c r="AF32" s="43"/>
+      <c r="AG32" s="43"/>
+      <c r="AH32" s="43"/>
+      <c r="AI32" s="43"/>
+      <c r="AJ32" s="43"/>
+      <c r="AK32" s="43"/>
+      <c r="AL32" s="43"/>
+      <c r="AM32" s="43"/>
+      <c r="AN32" s="43"/>
+      <c r="AO32" s="43"/>
+      <c r="AP32" s="43"/>
+      <c r="AQ32" s="43"/>
+      <c r="AR32" s="43"/>
+      <c r="AS32" s="43"/>
+      <c r="AT32" s="43"/>
+      <c r="AU32" s="43"/>
+      <c r="AV32" s="43"/>
+      <c r="AW32" s="43"/>
+      <c r="AX32" s="43"/>
+      <c r="AY32" s="43"/>
+      <c r="AZ32" s="43"/>
+      <c r="BA32" s="43"/>
+      <c r="BB32" s="43"/>
+      <c r="BC32" s="43"/>
+      <c r="BD32" s="43"/>
+      <c r="BE32" s="43"/>
+      <c r="BF32" s="43"/>
+      <c r="BG32" s="43"/>
+      <c r="BH32" s="43"/>
+      <c r="BI32" s="43"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="21"/>
+      <c r="BL32" s="21"/>
+    </row>
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
+      <c r="B33" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="52">
+        <v>0</v>
+      </c>
+      <c r="E33" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F33" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G33" s="66"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="43"/>
+      <c r="V33" s="43"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="43"/>
+      <c r="Y33" s="43"/>
+      <c r="Z33" s="43"/>
+      <c r="AA33" s="43"/>
+      <c r="AB33" s="43"/>
+      <c r="AC33" s="43"/>
+      <c r="AD33" s="43"/>
+      <c r="AE33" s="43"/>
+      <c r="AF33" s="43"/>
+      <c r="AG33" s="43"/>
+      <c r="AH33" s="43"/>
+      <c r="AI33" s="43"/>
+      <c r="AJ33" s="43"/>
+      <c r="AK33" s="43"/>
+      <c r="AL33" s="43"/>
+      <c r="AM33" s="43"/>
+      <c r="AN33" s="43"/>
+      <c r="AO33" s="43"/>
+      <c r="AP33" s="43"/>
+      <c r="AQ33" s="43"/>
+      <c r="AR33" s="43"/>
+      <c r="AS33" s="43"/>
+      <c r="AT33" s="43"/>
+      <c r="AU33" s="43"/>
+      <c r="AV33" s="43"/>
+      <c r="AW33" s="43"/>
+      <c r="AX33" s="43"/>
+      <c r="AY33" s="43"/>
+      <c r="AZ33" s="43"/>
+      <c r="BA33" s="43"/>
+      <c r="BB33" s="43"/>
+      <c r="BC33" s="43"/>
+      <c r="BD33" s="43"/>
+      <c r="BE33" s="43"/>
+      <c r="BF33" s="43"/>
+      <c r="BG33" s="43"/>
+      <c r="BH33" s="43"/>
+      <c r="BI33" s="43"/>
+      <c r="BJ33" s="21"/>
+      <c r="BK33" s="21"/>
+      <c r="BL33" s="21"/>
+    </row>
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="52">
+        <v>0</v>
+      </c>
+      <c r="E34" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F34" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G34" s="66"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="43"/>
+      <c r="T34" s="43"/>
+      <c r="U34" s="43"/>
+      <c r="V34" s="43"/>
+      <c r="W34" s="43"/>
+      <c r="X34" s="43"/>
+      <c r="Y34" s="43"/>
+      <c r="Z34" s="43"/>
+      <c r="AA34" s="43"/>
+      <c r="AB34" s="43"/>
+      <c r="AC34" s="43"/>
+      <c r="AD34" s="43"/>
+      <c r="AE34" s="43"/>
+      <c r="AF34" s="43"/>
+      <c r="AG34" s="43"/>
+      <c r="AH34" s="43"/>
+      <c r="AI34" s="43"/>
+      <c r="AJ34" s="43"/>
+      <c r="AK34" s="43"/>
+      <c r="AL34" s="43"/>
+      <c r="AM34" s="43"/>
+      <c r="AN34" s="43"/>
+      <c r="AO34" s="43"/>
+      <c r="AP34" s="43"/>
+      <c r="AQ34" s="43"/>
+      <c r="AR34" s="43"/>
+      <c r="AS34" s="43"/>
+      <c r="AT34" s="43"/>
+      <c r="AU34" s="43"/>
+      <c r="AV34" s="43"/>
+      <c r="AW34" s="43"/>
+      <c r="AX34" s="43"/>
+      <c r="AY34" s="43"/>
+      <c r="AZ34" s="43"/>
+      <c r="BA34" s="43"/>
+      <c r="BB34" s="43"/>
+      <c r="BC34" s="43"/>
+      <c r="BD34" s="43"/>
+      <c r="BE34" s="43"/>
+      <c r="BF34" s="43"/>
+      <c r="BG34" s="43"/>
+      <c r="BH34" s="43"/>
+      <c r="BI34" s="43"/>
+      <c r="BJ34" s="21"/>
+      <c r="BK34" s="21"/>
+      <c r="BL34" s="21"/>
+    </row>
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="52">
+        <v>0</v>
+      </c>
+      <c r="E35" s="53">
+        <v>44303</v>
+      </c>
+      <c r="F35" s="53">
+        <v>44316</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="43"/>
+      <c r="T35" s="43"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="43"/>
+      <c r="X35" s="43"/>
+      <c r="Y35" s="43"/>
+      <c r="Z35" s="43"/>
+      <c r="AA35" s="43"/>
+      <c r="AB35" s="43"/>
+      <c r="AC35" s="43"/>
+      <c r="AD35" s="43"/>
+      <c r="AE35" s="43"/>
+      <c r="AF35" s="43"/>
+      <c r="AG35" s="43"/>
+      <c r="AH35" s="43"/>
+      <c r="AI35" s="43"/>
+      <c r="AJ35" s="43"/>
+      <c r="AK35" s="43"/>
+      <c r="AL35" s="43"/>
+      <c r="AM35" s="43"/>
+      <c r="AN35" s="43"/>
+      <c r="AO35" s="43"/>
+      <c r="AP35" s="43"/>
+      <c r="AQ35" s="43"/>
+      <c r="AR35" s="43"/>
+      <c r="AS35" s="43"/>
+      <c r="AT35" s="43"/>
+      <c r="AU35" s="43"/>
+      <c r="AV35" s="43"/>
+      <c r="AW35" s="43"/>
+      <c r="AX35" s="43"/>
+      <c r="AY35" s="43"/>
+      <c r="AZ35" s="43"/>
+      <c r="BA35" s="43"/>
+      <c r="BB35" s="43"/>
+      <c r="BC35" s="43"/>
+      <c r="BD35" s="43"/>
+      <c r="BE35" s="43"/>
+      <c r="BF35" s="43"/>
+      <c r="BG35" s="43"/>
+      <c r="BH35" s="43"/>
+      <c r="BI35" s="43"/>
+      <c r="BJ35" s="21"/>
+      <c r="BK35" s="21"/>
+      <c r="BL35" s="21"/>
+    </row>
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B36" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20" t="str">
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="22"/>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="22"/>
-      <c r="Z22" s="22"/>
-      <c r="AA22" s="22"/>
-      <c r="AB22" s="22"/>
-      <c r="AC22" s="22"/>
-      <c r="AD22" s="22"/>
-      <c r="AE22" s="22"/>
-      <c r="AF22" s="22"/>
-      <c r="AG22" s="22"/>
-      <c r="AH22" s="22"/>
-      <c r="AI22" s="22"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="22"/>
-      <c r="AL22" s="22"/>
-      <c r="AM22" s="22"/>
-      <c r="AN22" s="22"/>
-      <c r="AO22" s="22"/>
-      <c r="AP22" s="22"/>
-      <c r="AQ22" s="22"/>
-      <c r="AR22" s="22"/>
-      <c r="AS22" s="22"/>
-      <c r="AT22" s="22"/>
-      <c r="AU22" s="22"/>
-      <c r="AV22" s="22"/>
-      <c r="AW22" s="22"/>
-      <c r="AX22" s="22"/>
-      <c r="AY22" s="22"/>
-      <c r="AZ22" s="22"/>
-      <c r="BA22" s="22"/>
-      <c r="BB22" s="22"/>
-      <c r="BC22" s="22"/>
-      <c r="BD22" s="22"/>
-      <c r="BE22" s="22"/>
-      <c r="BF22" s="22"/>
-      <c r="BG22" s="22"/>
-      <c r="BH22" s="22"/>
-      <c r="BI22" s="22"/>
-      <c r="BJ22" s="22"/>
-      <c r="BK22" s="22"/>
-      <c r="BL22" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="22"/>
+      <c r="AB36" s="22"/>
+      <c r="AC36" s="22"/>
+      <c r="AD36" s="22"/>
+      <c r="AE36" s="22"/>
+      <c r="AF36" s="22"/>
+      <c r="AG36" s="22"/>
+      <c r="AH36" s="22"/>
+      <c r="AI36" s="22"/>
+      <c r="AJ36" s="22"/>
+      <c r="AK36" s="22"/>
+      <c r="AL36" s="22"/>
+      <c r="AM36" s="22"/>
+      <c r="AN36" s="22"/>
+      <c r="AO36" s="22"/>
+      <c r="AP36" s="22"/>
+      <c r="AQ36" s="22"/>
+      <c r="AR36" s="22"/>
+      <c r="AS36" s="22"/>
+      <c r="AT36" s="22"/>
+      <c r="AU36" s="22"/>
+      <c r="AV36" s="22"/>
+      <c r="AW36" s="22"/>
+      <c r="AX36" s="22"/>
+      <c r="AY36" s="22"/>
+      <c r="AZ36" s="22"/>
+      <c r="BA36" s="22"/>
+      <c r="BB36" s="22"/>
+      <c r="BC36" s="22"/>
+      <c r="BD36" s="22"/>
+      <c r="BE36" s="22"/>
+      <c r="BF36" s="22"/>
+      <c r="BG36" s="22"/>
+      <c r="BH36" s="22"/>
+      <c r="BI36" s="22"/>
+      <c r="BJ36" s="22"/>
+      <c r="BK36" s="22"/>
+      <c r="BL36" s="22"/>
     </row>
-    <row r="23" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="6"/>
+    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="6"/>
     </row>
-    <row r="24" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
-      <c r="F24" s="26"/>
+    <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="11"/>
+      <c r="F38" s="26"/>
     </row>
-    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="12"/>
+    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3496,8 +4655,8 @@
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D9 D22 D11 D18:D20">
-    <cfRule type="dataBar" priority="28">
+  <conditionalFormatting sqref="D7:D9 D36 D11 D19 D24">
+    <cfRule type="dataBar" priority="84">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3510,21 +4669,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL22">
-    <cfRule type="expression" dxfId="2" priority="47">
+  <conditionalFormatting sqref="I5:BL36">
+    <cfRule type="expression" dxfId="2" priority="103">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL22">
-    <cfRule type="expression" dxfId="1" priority="41">
+  <conditionalFormatting sqref="I7:BL36">
+    <cfRule type="expression" dxfId="1" priority="97">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="98" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D20 D10:D11">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="dataBar" priority="65">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3538,7 +4697,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3552,7 +4711,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3565,8 +4724,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15 D17">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="D16 D18">
+    <cfRule type="dataBar" priority="62">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3579,8 +4738,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D17">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="D17:D18">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3594,7 +4753,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="60">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3607,7 +4766,581 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="D13:D14">
+    <cfRule type="dataBar" priority="57">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8869D331-A7CF-4870-8E9C-A0823634313E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="dataBar" priority="54">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D448656C-2190-4E81-A11B-96B46A35E718}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="dataBar" priority="53">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{321F1F73-7B48-48D1-8638-A867BBD94D60}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="dataBar" priority="52">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1B75D785-0386-4856-98AB-48D81809E739}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="dataBar" priority="51">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{444CC7AF-8CC1-4332-96E2-39B6F996D06F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="dataBar" priority="50">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4758CAAE-4C07-4C39-91FD-C78221C45293}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="dataBar" priority="49">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5407EF65-B65F-4841-AC26-F129E0BF7696}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="dataBar" priority="48">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{712E70AC-1366-47D9-A531-AD112E4AB6F8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D22">
+    <cfRule type="dataBar" priority="47">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E359F141-7A2D-487F-9A2A-0FFADA228248}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="dataBar" priority="44">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CC7A7095-E211-42E2-BB98-61211C66C22F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="dataBar" priority="43">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FA36ACE5-0BA5-4EBC-A26A-404FD08BD865}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="dataBar" priority="42">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C9993970-427E-4641-A58B-E53A0A0BAC82}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="dataBar" priority="41">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9389D3AE-C7A5-4443-8F6B-702A837B3679}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="dataBar" priority="40">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3DEE4854-B726-4428-8A4E-60C5F9672B5C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="dataBar" priority="31">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BB7BC8D0-EB93-417A-9BCA-87D3D5427AB2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29">
+    <cfRule type="dataBar" priority="32">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9C9D4A15-5744-43C4-93DB-A6B8678B9A08}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D33">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CDE2337F-565A-4463-B682-D15CA2647C94}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="dataBar" priority="36">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6E450BBB-3D02-4C70-96F9-9752BEE7C982}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28">
+    <cfRule type="dataBar" priority="35">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AA2FAFFA-EC2C-459C-8D54-A0DFE82086A9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="dataBar" priority="30">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0E993CC7-399A-4C52-ACAB-BEECC816F4DF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="dataBar" priority="29">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{52230AB8-3070-4A11-821B-F2403C9AA9BF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D33">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{34B290CB-1471-4F0E-B332-A2693AC854C6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{ADD2E25D-1593-451D-BF4F-494D76FE2BAC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D31">
+    <cfRule type="dataBar" priority="28">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D114266E-DCFD-490E-B6AF-B4593493EE30}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D31">
+    <cfRule type="dataBar" priority="27">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{680EFF7E-0FED-4298-90DD-6F0F63ED4A05}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{906C9A53-D4F1-4E6A-BA03-D7D75F13D629}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2CF9745F-338A-4B44-BE91-2A1B1559A9A9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{679A023A-C2A0-41A7-9D8E-3E17253DC6F1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0BC38917-7F43-4FDA-9C25-B487537A13AA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D33">
+    <cfRule type="dataBar" priority="24">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C259914D-3D04-4DEE-81A6-2E8DE5BFDFBC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D33">
+    <cfRule type="dataBar" priority="23">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6321DED7-A12A-41C1-979F-A1124F0FA7BF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D74BED5F-7116-40CC-A4D1-61311B04F835}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D0972F16-73C9-4A2E-B520-8F221A015C62}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AE0DBD5C-8468-4D5A-B9F3-401B50C12A1E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{12DD82C2-8CF8-44E6-B4A6-986E3DFCAA5B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1E2CA01B-C885-4B1B-BDAC-867236E441C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1723A971-90BD-4903-AE9E-378A023BABFE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4082F14F-772E-4E73-88DD-ECDF3475480F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1712A78B-5806-460E-8F16-343646BF490C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{18DAFC6D-9391-4FFD-9844-A9606E70A44F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{83CC43A2-3757-497C-AE47-023D422DE77D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -3616,7 +5349,63 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8869D331-A7CF-4870-8E9C-A0823634313E}</x14:id>
+          <x14:id>{474B52C7-F05E-484C-AE4A-7B839432ECC5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{13FBE554-EF1C-4F9F-9C79-CDA8BF51BB3C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F6262373-9022-4846-A0A7-0503744D09E2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{25BF47B7-FDB3-45FE-905A-B91AC0BA472D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AB54FE81-C321-4B4A-B6E0-6742B469016C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3648,7 +5437,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D9 D22 D11 D18:D20</xm:sqref>
+          <xm:sqref>D7:D9 D36 D11 D19 D24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6A02471B-CBED-420D-A71B-22E39791D61B}">
@@ -3663,7 +5452,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D18:D20 D10:D11</xm:sqref>
+          <xm:sqref>D10:D11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{606330BC-8714-4A7C-9BE9-776CF1EFC90A}">
@@ -3708,7 +5497,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15 D17</xm:sqref>
+          <xm:sqref>D16 D18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09394F4F-D07D-40CB-9B4B-8B70D7C3FAF3}">
@@ -3723,7 +5512,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D16:D17</xm:sqref>
+          <xm:sqref>D17:D18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CC63ED0A-E798-4FE3-AFB5-F7034939D379}">
@@ -3753,7 +5542,682 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D13</xm:sqref>
+          <xm:sqref>D13:D14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D448656C-2190-4E81-A11B-96B46A35E718}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{321F1F73-7B48-48D1-8638-A867BBD94D60}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1B75D785-0386-4856-98AB-48D81809E739}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{444CC7AF-8CC1-4332-96E2-39B6F996D06F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4758CAAE-4C07-4C39-91FD-C78221C45293}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5407EF65-B65F-4841-AC26-F129E0BF7696}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{712E70AC-1366-47D9-A531-AD112E4AB6F8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E359F141-7A2D-487F-9A2A-0FFADA228248}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D21:D22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CC7A7095-E211-42E2-BB98-61211C66C22F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FA36ACE5-0BA5-4EBC-A26A-404FD08BD865}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C9993970-427E-4641-A58B-E53A0A0BAC82}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9389D3AE-C7A5-4443-8F6B-702A837B3679}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3DEE4854-B726-4428-8A4E-60C5F9672B5C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BB7BC8D0-EB93-417A-9BCA-87D3D5427AB2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9C9D4A15-5744-43C4-93DB-A6B8678B9A08}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CDE2337F-565A-4463-B682-D15CA2647C94}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32:D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6E450BBB-3D02-4C70-96F9-9752BEE7C982}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AA2FAFFA-EC2C-459C-8D54-A0DFE82086A9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0E993CC7-399A-4C52-ACAB-BEECC816F4DF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{52230AB8-3070-4A11-821B-F2403C9AA9BF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{34B290CB-1471-4F0E-B332-A2693AC854C6}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32:D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{ADD2E25D-1593-451D-BF4F-494D76FE2BAC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D114266E-DCFD-490E-B6AF-B4593493EE30}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D30:D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{680EFF7E-0FED-4298-90DD-6F0F63ED4A05}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D30:D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{906C9A53-D4F1-4E6A-BA03-D7D75F13D629}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2CF9745F-338A-4B44-BE91-2A1B1559A9A9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{679A023A-C2A0-41A7-9D8E-3E17253DC6F1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0BC38917-7F43-4FDA-9C25-B487537A13AA}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C259914D-3D04-4DEE-81A6-2E8DE5BFDFBC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32:D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6321DED7-A12A-41C1-979F-A1124F0FA7BF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32:D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D74BED5F-7116-40CC-A4D1-61311B04F835}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D0972F16-73C9-4A2E-B520-8F221A015C62}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AE0DBD5C-8468-4D5A-B9F3-401B50C12A1E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{12DD82C2-8CF8-44E6-B4A6-986E3DFCAA5B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1E2CA01B-C885-4B1B-BDAC-867236E441C3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1723A971-90BD-4903-AE9E-378A023BABFE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4082F14F-772E-4E73-88DD-ECDF3475480F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1712A78B-5806-460E-8F16-343646BF490C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{18DAFC6D-9391-4FFD-9844-A9606E70A44F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{83CC43A2-3757-497C-AE47-023D422DE77D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{474B52C7-F05E-484C-AE4A-7B839432ECC5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{13FBE554-EF1C-4F9F-9C79-CDA8BF51BB3C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F6262373-9022-4846-A0A7-0503744D09E2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{25BF47B7-FDB3-45FE-905A-B91AC0BA472D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AB54FE81-C321-4B4A-B6E0-6742B469016C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Woche 4 Sprint Planung
</commit_message>
<xml_diff>
--- a/Projektleiter/GanttChart_4_Semester.xlsx
+++ b/Projektleiter/GanttChart_4_Semester.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30413701-5EAC-416B-9073-171C9A7D06C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4C49E6-0C2F-46BF-9325-E01696B95FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -1200,7 +1200,55 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="43" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="43" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="44" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="44" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="44" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="45" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="46" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,55 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="43" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="43" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="43" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="43" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="44" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="44" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="44" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="45" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="46" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:BL39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1871,105 +1871,105 @@
       <c r="D3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="83">
         <v>44263</v>
       </c>
-      <c r="F3" s="62"/>
+      <c r="F3" s="83"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="66"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="46" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="79">
         <f>I5</f>
         <v>44263</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="63">
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="79">
         <f>P5</f>
         <v>44270</v>
       </c>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="63">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="79">
         <f>W5</f>
         <v>44277</v>
       </c>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="65"/>
-      <c r="AD4" s="63">
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="79">
         <f>AD5</f>
         <v>44284</v>
       </c>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="65"/>
-      <c r="AK4" s="63">
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="79">
         <f>AK5</f>
         <v>44291</v>
       </c>
-      <c r="AL4" s="64"/>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="65"/>
-      <c r="AR4" s="63">
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="79">
         <f>AR5</f>
         <v>44298</v>
       </c>
-      <c r="AS4" s="64"/>
-      <c r="AT4" s="64"/>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="65"/>
-      <c r="AY4" s="63">
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="79">
         <f>AY5</f>
         <v>44305</v>
       </c>
-      <c r="AZ4" s="64"/>
-      <c r="BA4" s="64"/>
-      <c r="BB4" s="64"/>
-      <c r="BC4" s="64"/>
-      <c r="BD4" s="64"/>
-      <c r="BE4" s="65"/>
-      <c r="BF4" s="63">
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="79">
         <f>BF5</f>
         <v>44312</v>
       </c>
-      <c r="BG4" s="64"/>
-      <c r="BH4" s="64"/>
-      <c r="BI4" s="64"/>
-      <c r="BJ4" s="64"/>
-      <c r="BK4" s="64"/>
-      <c r="BL4" s="65"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="80"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="81"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
@@ -3507,13 +3507,13 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="43"/>
@@ -3575,19 +3575,19 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="73">
+      <c r="D22" s="68">
         <v>0</v>
       </c>
-      <c r="E22" s="74">
+      <c r="E22" s="69">
         <v>44291</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="69">
         <v>44302</v>
       </c>
       <c r="G22" s="13"/>
@@ -3651,19 +3651,19 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="75">
+      <c r="D23" s="70">
         <v>0</v>
       </c>
-      <c r="E23" s="74">
+      <c r="E23" s="69">
         <v>44291</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="69">
         <v>44302</v>
       </c>
       <c r="G23" s="13"/>
@@ -3727,19 +3727,19 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="75">
+      <c r="D24" s="70">
         <v>0</v>
       </c>
-      <c r="E24" s="74">
+      <c r="E24" s="69">
         <v>44291</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F24" s="69">
         <v>44302</v>
       </c>
       <c r="G24" s="13"/>
@@ -3803,13 +3803,13 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="43"/>
@@ -3871,19 +3871,19 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="78">
+      <c r="D26" s="73">
         <v>0</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="74">
         <v>44303</v>
       </c>
-      <c r="F26" s="79">
+      <c r="F26" s="74">
         <v>44316</v>
       </c>
       <c r="G26" s="13"/>
@@ -3947,19 +3947,19 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="78">
+      <c r="D27" s="73">
         <v>0</v>
       </c>
-      <c r="E27" s="79">
+      <c r="E27" s="74">
         <v>44303</v>
       </c>
-      <c r="F27" s="79">
+      <c r="F27" s="74">
         <v>44316</v>
       </c>
       <c r="G27" s="13"/>
@@ -4023,19 +4023,19 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="78">
+      <c r="D28" s="73">
         <v>0</v>
       </c>
-      <c r="E28" s="79">
+      <c r="E28" s="74">
         <v>44303</v>
       </c>
-      <c r="F28" s="79">
+      <c r="F28" s="74">
         <v>44316</v>
       </c>
       <c r="G28" s="13"/>
@@ -4099,19 +4099,19 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="78">
+      <c r="D29" s="73">
         <v>0</v>
       </c>
-      <c r="E29" s="79">
+      <c r="E29" s="74">
         <v>44303</v>
       </c>
-      <c r="F29" s="79">
+      <c r="F29" s="74">
         <v>44316</v>
       </c>
       <c r="G29" s="61"/>
@@ -4175,19 +4175,19 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25"/>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="78">
+      <c r="D30" s="73">
         <v>0</v>
       </c>
-      <c r="E30" s="79">
+      <c r="E30" s="74">
         <v>44303</v>
       </c>
-      <c r="F30" s="79">
+      <c r="F30" s="74">
         <v>44316</v>
       </c>
       <c r="G30" s="61"/>
@@ -4251,19 +4251,19 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25"/>
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="78">
+      <c r="D31" s="73">
         <v>0</v>
       </c>
-      <c r="E31" s="79">
+      <c r="E31" s="74">
         <v>44303</v>
       </c>
-      <c r="F31" s="79">
+      <c r="F31" s="74">
         <v>44316</v>
       </c>
       <c r="G31" s="61"/>
@@ -4327,19 +4327,19 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="78">
+      <c r="D32" s="73">
         <v>0</v>
       </c>
-      <c r="E32" s="79">
+      <c r="E32" s="74">
         <v>44303</v>
       </c>
-      <c r="F32" s="79">
+      <c r="F32" s="74">
         <v>44316</v>
       </c>
       <c r="G32" s="61"/>
@@ -4403,19 +4403,19 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25"/>
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="78">
+      <c r="D33" s="73">
         <v>0</v>
       </c>
-      <c r="E33" s="79">
+      <c r="E33" s="74">
         <v>44303</v>
       </c>
-      <c r="F33" s="79">
+      <c r="F33" s="74">
         <v>44316</v>
       </c>
       <c r="G33" s="61"/>
@@ -4479,19 +4479,19 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25"/>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="77" t="s">
+      <c r="C34" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="78">
+      <c r="D34" s="73">
         <v>0</v>
       </c>
-      <c r="E34" s="79">
+      <c r="E34" s="74">
         <v>44303</v>
       </c>
-      <c r="F34" s="79">
+      <c r="F34" s="74">
         <v>44316</v>
       </c>
       <c r="G34" s="61"/>
@@ -4557,19 +4557,19 @@
       <c r="A35" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="77" t="s">
+      <c r="C35" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="78">
+      <c r="D35" s="73">
         <v>0</v>
       </c>
-      <c r="E35" s="79">
+      <c r="E35" s="74">
         <v>44303</v>
       </c>
-      <c r="F35" s="79">
+      <c r="F35" s="74">
         <v>44316</v>
       </c>
       <c r="G35" s="13"/>
@@ -4719,16 +4719,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D9 D36 D11 D19 D24">
     <cfRule type="dataBar" priority="84">

</xml_diff>

<commit_message>
Finaler Push aller lokaler Dateien PM
</commit_message>
<xml_diff>
--- a/Projektleiter/GanttChart_4_Semester.xlsx
+++ b/Projektleiter/GanttChart_4_Semester.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CE30FA-0439-4216-AB0D-C52E2F15B841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DAC571-2DB8-4FC4-8B10-86CACDB4A24B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17790" yWindow="1920" windowWidth="21600" windowHeight="11385" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -89,12 +89,6 @@
 Von Zelle I9 bis Zelle BL9 wird eine Statusleiste mit einer entsprechenden Schattierung für die eingegebenen Datumsangaben in Blöcken angezeigt. </t>
   </si>
   <si>
-    <t>In den Zeilen 10 bis 13 wird das Muster aus Zeile 9 wiederholt. 
-Wiederholen Sie die Anweisungen aus Zelle A9 für alle Aufgabenzeilen auf diesem Arbeitsblatt. Überschreiben Sie alle Beispieldaten.
-Ein Beispiel für eine andere Phase beginnt in Zelle A14. 
-Setzen Sie die Eingabe von Aufgaben in den Zellen A10 bis A13 fort, oder wechseln Sie zu Zelle A14, um weitere Informationen zu erhalten.</t>
-  </si>
-  <si>
     <t>Diese Zeile kennzeichnet das Ende des Projektplans. Geben Sie in dieser Zeile NICHTS EIN. 
 Fügen Sie ÜBER dieser Zeile neue Zeilen ein, um mit der Erstellung Ihres Projektplans fortzufahren.</t>
   </si>
@@ -214,9 +208,6 @@
     <t>Non-Functional: NF100</t>
   </si>
   <si>
-    <t>Functional:  F50, F80</t>
-  </si>
-  <si>
     <t>Functional: F30, F60, F40</t>
   </si>
   <si>
@@ -263,6 +254,39 @@
   </si>
   <si>
     <t>SJ</t>
+  </si>
+  <si>
+    <t>5 Sprint</t>
+  </si>
+  <si>
+    <t>Functional:  F50</t>
+  </si>
+  <si>
+    <t>Issues Umbennen</t>
+  </si>
+  <si>
+    <t>TZ, JS</t>
+  </si>
+  <si>
+    <t>Docstrings hinzufügen</t>
+  </si>
+  <si>
+    <t>Finale Produktpräsentation vorbereiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLE </t>
+  </si>
+  <si>
+    <t>6 Sprint</t>
+  </si>
+  <si>
+    <t>Homepage des Wikis anpassen</t>
+  </si>
+  <si>
+    <t>Abgabevorbereitungen</t>
+  </si>
+  <si>
+    <t>ALLE</t>
   </si>
 </sst>
 </file>
@@ -494,7 +518,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +782,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -1031,7 +1067,7 @@
     <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1151,9 +1187,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1"/>
@@ -1249,6 +1282,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="45" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="47" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="47" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="48" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="48" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="48" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="48" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="171" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
@@ -1817,11 +1877,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL39"/>
+  <dimension ref="A1:BL46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1857,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="27"/>
     </row>
@@ -1866,344 +1926,344 @@
         <v>2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="79">
+        <v>21</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="87">
         <v>44263</v>
       </c>
-      <c r="F3" s="79"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="46" t="s">
-        <v>19</v>
+      <c r="B4" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="91"/>
+      <c r="D4" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="80">
+        <v>3</v>
+      </c>
+      <c r="I4" s="88">
         <f>I5</f>
-        <v>44263</v>
-      </c>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="80">
+        <v>44277</v>
+      </c>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f>P5</f>
-        <v>44270</v>
-      </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="80">
+        <v>44284</v>
+      </c>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f>W5</f>
-        <v>44277</v>
-      </c>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="81"/>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="80">
+        <v>44291</v>
+      </c>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f>AD5</f>
-        <v>44284</v>
-      </c>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="81"/>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="82"/>
-      <c r="AK4" s="80">
+        <v>44298</v>
+      </c>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f>AK5</f>
-        <v>44291</v>
-      </c>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="81"/>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="82"/>
-      <c r="AR4" s="80">
+        <v>44305</v>
+      </c>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f>AR5</f>
-        <v>44298</v>
-      </c>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="81"/>
-      <c r="AU4" s="81"/>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="82"/>
-      <c r="AY4" s="80">
+        <v>44312</v>
+      </c>
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f>AY5</f>
-        <v>44305</v>
-      </c>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="81"/>
-      <c r="BB4" s="81"/>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="82"/>
-      <c r="BF4" s="80">
+        <v>44319</v>
+      </c>
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f>BF5</f>
-        <v>44312</v>
-      </c>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="81"/>
-      <c r="BI4" s="81"/>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="82"/>
+        <v>44326</v>
+      </c>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="I5" s="40">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Woche_anzeigen-1)</f>
-        <v>44263</v>
+        <v>44277</v>
       </c>
       <c r="J5" s="41">
         <f>I5+1</f>
-        <v>44264</v>
+        <v>44278</v>
       </c>
       <c r="K5" s="41">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>44265</v>
+        <v>44279</v>
       </c>
       <c r="L5" s="41">
         <f t="shared" si="0"/>
-        <v>44266</v>
+        <v>44280</v>
       </c>
       <c r="M5" s="41">
         <f t="shared" si="0"/>
-        <v>44267</v>
+        <v>44281</v>
       </c>
       <c r="N5" s="41">
         <f t="shared" si="0"/>
-        <v>44268</v>
+        <v>44282</v>
       </c>
       <c r="O5" s="42">
         <f t="shared" si="0"/>
-        <v>44269</v>
+        <v>44283</v>
       </c>
       <c r="P5" s="40">
         <f>O5+1</f>
-        <v>44270</v>
+        <v>44284</v>
       </c>
       <c r="Q5" s="41">
         <f>P5+1</f>
-        <v>44271</v>
+        <v>44285</v>
       </c>
       <c r="R5" s="41">
         <f t="shared" si="0"/>
-        <v>44272</v>
+        <v>44286</v>
       </c>
       <c r="S5" s="41">
         <f t="shared" si="0"/>
-        <v>44273</v>
+        <v>44287</v>
       </c>
       <c r="T5" s="41">
         <f t="shared" si="0"/>
-        <v>44274</v>
+        <v>44288</v>
       </c>
       <c r="U5" s="41">
         <f t="shared" si="0"/>
-        <v>44275</v>
+        <v>44289</v>
       </c>
       <c r="V5" s="42">
         <f t="shared" si="0"/>
-        <v>44276</v>
+        <v>44290</v>
       </c>
       <c r="W5" s="40">
         <f>V5+1</f>
-        <v>44277</v>
+        <v>44291</v>
       </c>
       <c r="X5" s="41">
         <f>W5+1</f>
-        <v>44278</v>
+        <v>44292</v>
       </c>
       <c r="Y5" s="41">
         <f t="shared" si="0"/>
-        <v>44279</v>
+        <v>44293</v>
       </c>
       <c r="Z5" s="41">
         <f t="shared" si="0"/>
-        <v>44280</v>
+        <v>44294</v>
       </c>
       <c r="AA5" s="41">
         <f t="shared" si="0"/>
-        <v>44281</v>
+        <v>44295</v>
       </c>
       <c r="AB5" s="41">
         <f t="shared" si="0"/>
-        <v>44282</v>
+        <v>44296</v>
       </c>
       <c r="AC5" s="42">
         <f t="shared" si="0"/>
-        <v>44283</v>
+        <v>44297</v>
       </c>
       <c r="AD5" s="40">
         <f>AC5+1</f>
-        <v>44284</v>
+        <v>44298</v>
       </c>
       <c r="AE5" s="41">
         <f>AD5+1</f>
-        <v>44285</v>
+        <v>44299</v>
       </c>
       <c r="AF5" s="41">
         <f t="shared" si="0"/>
-        <v>44286</v>
+        <v>44300</v>
       </c>
       <c r="AG5" s="41">
         <f t="shared" si="0"/>
-        <v>44287</v>
+        <v>44301</v>
       </c>
       <c r="AH5" s="41">
         <f t="shared" si="0"/>
-        <v>44288</v>
+        <v>44302</v>
       </c>
       <c r="AI5" s="41">
         <f t="shared" si="0"/>
-        <v>44289</v>
+        <v>44303</v>
       </c>
       <c r="AJ5" s="42">
         <f t="shared" si="0"/>
-        <v>44290</v>
+        <v>44304</v>
       </c>
       <c r="AK5" s="40">
         <f>AJ5+1</f>
-        <v>44291</v>
+        <v>44305</v>
       </c>
       <c r="AL5" s="41">
         <f>AK5+1</f>
-        <v>44292</v>
+        <v>44306</v>
       </c>
       <c r="AM5" s="41">
         <f t="shared" si="0"/>
-        <v>44293</v>
+        <v>44307</v>
       </c>
       <c r="AN5" s="41">
         <f t="shared" si="0"/>
-        <v>44294</v>
+        <v>44308</v>
       </c>
       <c r="AO5" s="41">
         <f t="shared" si="0"/>
-        <v>44295</v>
+        <v>44309</v>
       </c>
       <c r="AP5" s="41">
         <f t="shared" si="0"/>
-        <v>44296</v>
+        <v>44310</v>
       </c>
       <c r="AQ5" s="42">
         <f t="shared" si="0"/>
-        <v>44297</v>
+        <v>44311</v>
       </c>
       <c r="AR5" s="40">
         <f>AQ5+1</f>
-        <v>44298</v>
+        <v>44312</v>
       </c>
       <c r="AS5" s="41">
         <f>AR5+1</f>
-        <v>44299</v>
+        <v>44313</v>
       </c>
       <c r="AT5" s="41">
         <f t="shared" si="0"/>
-        <v>44300</v>
+        <v>44314</v>
       </c>
       <c r="AU5" s="41">
         <f t="shared" si="0"/>
-        <v>44301</v>
+        <v>44315</v>
       </c>
       <c r="AV5" s="41">
         <f t="shared" si="0"/>
-        <v>44302</v>
+        <v>44316</v>
       </c>
       <c r="AW5" s="41">
         <f t="shared" si="0"/>
-        <v>44303</v>
+        <v>44317</v>
       </c>
       <c r="AX5" s="42">
         <f t="shared" si="0"/>
-        <v>44304</v>
+        <v>44318</v>
       </c>
       <c r="AY5" s="40">
         <f>AX5+1</f>
-        <v>44305</v>
+        <v>44319</v>
       </c>
       <c r="AZ5" s="41">
         <f>AY5+1</f>
-        <v>44306</v>
+        <v>44320</v>
       </c>
       <c r="BA5" s="41">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>44307</v>
+        <v>44321</v>
       </c>
       <c r="BB5" s="41">
         <f t="shared" si="1"/>
-        <v>44308</v>
+        <v>44322</v>
       </c>
       <c r="BC5" s="41">
         <f t="shared" si="1"/>
-        <v>44309</v>
+        <v>44323</v>
       </c>
       <c r="BD5" s="41">
         <f t="shared" si="1"/>
-        <v>44310</v>
+        <v>44324</v>
       </c>
       <c r="BE5" s="42">
         <f t="shared" si="1"/>
-        <v>44311</v>
+        <v>44325</v>
       </c>
       <c r="BF5" s="40">
         <f>BE5+1</f>
-        <v>44312</v>
+        <v>44326</v>
       </c>
       <c r="BG5" s="41">
         <f>BF5+1</f>
-        <v>44313</v>
+        <v>44327</v>
       </c>
       <c r="BH5" s="41">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>44314</v>
+        <v>44328</v>
       </c>
       <c r="BI5" s="41">
         <f t="shared" si="2"/>
-        <v>44315</v>
+        <v>44329</v>
       </c>
       <c r="BJ5" s="41">
         <f t="shared" si="2"/>
-        <v>44316</v>
+        <v>44330</v>
       </c>
       <c r="BK5" s="41">
         <f t="shared" si="2"/>
-        <v>44317</v>
+        <v>44331</v>
       </c>
       <c r="BL5" s="42">
         <f t="shared" si="2"/>
-        <v>44318</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2211,23 +2271,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="10" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"TTT"),1)</f>
@@ -2526,7 +2586,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="15"/>
@@ -2534,7 +2594,7 @@
       <c r="F8" s="36"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="str">
-        <f t="shared" ref="H8:H36" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H43" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="43"/>
@@ -2599,10 +2659,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -2679,10 +2739,10 @@
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2756,10 +2816,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="16">
         <v>1</v>
@@ -2832,10 +2892,10 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="16">
         <v>1</v>
@@ -2908,10 +2968,10 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25"/>
       <c r="B13" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="16">
         <v>1</v>
@@ -2984,10 +3044,10 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
       <c r="B14" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>34</v>
       </c>
       <c r="D14" s="16">
         <v>1</v>
@@ -3060,10 +3120,10 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="16">
         <v>1</v>
@@ -3135,19 +3195,19 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="59">
+      <c r="D16" s="58">
         <v>1</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="59">
         <v>44281</v>
       </c>
-      <c r="F16" s="60">
+      <c r="F16" s="59">
         <v>44281</v>
       </c>
       <c r="G16" s="13"/>
@@ -3211,13 +3271,13 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25"/>
-      <c r="B17" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
+      <c r="B17" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="43"/>
@@ -3279,19 +3339,19 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="52">
+      <c r="B18" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="51">
         <v>1</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="52">
         <v>44281</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="52">
         <v>44289</v>
       </c>
       <c r="G18" s="13"/>
@@ -3355,19 +3415,19 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="54">
+      <c r="B19" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="53">
         <v>1</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="52">
         <v>44281</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="52">
         <v>44289</v>
       </c>
       <c r="G19" s="13"/>
@@ -3431,20 +3491,20 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="53">
+      <c r="D20" s="53">
+        <v>1</v>
+      </c>
+      <c r="E20" s="52">
         <v>44281</v>
       </c>
-      <c r="F20" s="53">
-        <v>44302</v>
+      <c r="F20" s="52">
+        <v>44323</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
@@ -3507,13 +3567,13 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
+      <c r="B21" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="43"/>
@@ -3575,19 +3635,19 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="68">
-        <v>0</v>
-      </c>
-      <c r="E22" s="69">
+      <c r="B22" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="67">
+        <v>1</v>
+      </c>
+      <c r="E22" s="68">
         <v>44291</v>
       </c>
-      <c r="F22" s="69">
+      <c r="F22" s="68">
         <v>44302</v>
       </c>
       <c r="G22" s="13"/>
@@ -3651,19 +3711,19 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
-      <c r="B23" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="70">
-        <v>0</v>
-      </c>
-      <c r="E23" s="69">
+      <c r="B23" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="69">
+        <v>1</v>
+      </c>
+      <c r="E23" s="68">
         <v>44291</v>
       </c>
-      <c r="F23" s="69">
+      <c r="F23" s="68">
         <v>44302</v>
       </c>
       <c r="G23" s="13"/>
@@ -3727,19 +3787,19 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
-      <c r="B24" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="70">
-        <v>0</v>
-      </c>
-      <c r="E24" s="69">
+      <c r="B24" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="69">
+        <v>1</v>
+      </c>
+      <c r="E24" s="68">
         <v>44291</v>
       </c>
-      <c r="F24" s="69">
+      <c r="F24" s="68">
         <v>44302</v>
       </c>
       <c r="G24" s="13"/>
@@ -3803,13 +3863,13 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
-      <c r="B25" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
+      <c r="B25" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="43"/>
@@ -3871,19 +3931,19 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
-      <c r="B26" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="73">
-        <v>0</v>
-      </c>
-      <c r="E26" s="74">
+      <c r="B26" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="72">
+        <v>1</v>
+      </c>
+      <c r="E26" s="73">
         <v>44303</v>
       </c>
-      <c r="F26" s="74">
+      <c r="F26" s="73">
         <v>44316</v>
       </c>
       <c r="G26" s="13"/>
@@ -3947,19 +4007,19 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
-      <c r="B27" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="73">
-        <v>0</v>
-      </c>
-      <c r="E27" s="74">
+      <c r="B27" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="72">
+        <v>1</v>
+      </c>
+      <c r="E27" s="73">
         <v>44303</v>
       </c>
-      <c r="F27" s="74">
+      <c r="F27" s="73">
         <v>44316</v>
       </c>
       <c r="G27" s="13"/>
@@ -4023,19 +4083,19 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="73">
-        <v>0</v>
-      </c>
-      <c r="E28" s="74">
+      <c r="D28" s="72">
+        <v>1</v>
+      </c>
+      <c r="E28" s="73">
         <v>44303</v>
       </c>
-      <c r="F28" s="74">
+      <c r="F28" s="73">
         <v>44316</v>
       </c>
       <c r="G28" s="13"/>
@@ -4099,22 +4159,22 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
-      <c r="B29" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="73">
-        <v>0</v>
-      </c>
-      <c r="E29" s="74">
+      <c r="B29" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="72">
+        <v>1</v>
+      </c>
+      <c r="E29" s="73">
         <v>44303</v>
       </c>
-      <c r="F29" s="74">
+      <c r="F29" s="73">
         <v>44316</v>
       </c>
-      <c r="G29" s="61"/>
+      <c r="G29" s="60"/>
       <c r="H29" s="13"/>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
@@ -4175,22 +4235,22 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25"/>
-      <c r="B30" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="73">
-        <v>0</v>
-      </c>
-      <c r="E30" s="74">
+      <c r="B30" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="72">
+        <v>1</v>
+      </c>
+      <c r="E30" s="73">
         <v>44303</v>
       </c>
-      <c r="F30" s="74">
+      <c r="F30" s="73">
         <v>44316</v>
       </c>
-      <c r="G30" s="61"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="13"/>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -4251,22 +4311,22 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25"/>
-      <c r="B31" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="73">
-        <v>0</v>
-      </c>
-      <c r="E31" s="74">
+      <c r="B31" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="72">
+        <v>1</v>
+      </c>
+      <c r="E31" s="73">
         <v>44303</v>
       </c>
-      <c r="F31" s="74">
-        <v>44316</v>
-      </c>
-      <c r="G31" s="61"/>
+      <c r="F31" s="73">
+        <v>44327</v>
+      </c>
+      <c r="G31" s="60"/>
       <c r="H31" s="13"/>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
@@ -4327,22 +4387,22 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
-      <c r="B32" s="71" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="73">
-        <v>0.8</v>
-      </c>
-      <c r="E32" s="74">
+      <c r="B32" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="72">
+        <v>1</v>
+      </c>
+      <c r="E32" s="73">
         <v>44303</v>
       </c>
-      <c r="F32" s="74">
-        <v>44316</v>
-      </c>
-      <c r="G32" s="61"/>
+      <c r="F32" s="73">
+        <v>44330</v>
+      </c>
+      <c r="G32" s="60"/>
       <c r="H32" s="13"/>
       <c r="I32" s="43"/>
       <c r="J32" s="43"/>
@@ -4403,22 +4463,22 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25"/>
-      <c r="B33" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="73">
-        <v>0</v>
-      </c>
-      <c r="E33" s="74">
+      <c r="B33" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="72">
+        <v>1</v>
+      </c>
+      <c r="E33" s="73">
         <v>44303</v>
       </c>
-      <c r="F33" s="74">
+      <c r="F33" s="73">
         <v>44316</v>
       </c>
-      <c r="G33" s="61"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="13"/>
       <c r="I33" s="43"/>
       <c r="J33" s="43"/>
@@ -4479,22 +4539,22 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25"/>
-      <c r="B34" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="73">
-        <v>0</v>
-      </c>
-      <c r="E34" s="74">
+      <c r="B34" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="72">
+        <v>1</v>
+      </c>
+      <c r="E34" s="73">
         <v>44303</v>
       </c>
-      <c r="F34" s="74">
+      <c r="F34" s="73">
         <v>44316</v>
       </c>
-      <c r="G34" s="61"/>
+      <c r="G34" s="60"/>
       <c r="H34" s="13"/>
       <c r="I34" s="43"/>
       <c r="J34" s="43"/>
@@ -4554,29 +4614,24 @@
       <c r="BL34" s="21"/>
     </row>
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="73">
-        <v>0</v>
-      </c>
-      <c r="E35" s="74">
+      <c r="A35" s="25"/>
+      <c r="B35" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="72">
+        <v>1</v>
+      </c>
+      <c r="E35" s="73">
         <v>44303</v>
       </c>
-      <c r="F35" s="74">
+      <c r="F35" s="73">
         <v>44316</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
+      <c r="G35" s="60"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
       <c r="K35" s="43"/>
@@ -4589,8 +4644,8 @@
       <c r="R35" s="43"/>
       <c r="S35" s="43"/>
       <c r="T35" s="43"/>
-      <c r="U35" s="44"/>
-      <c r="V35" s="44"/>
+      <c r="U35" s="43"/>
+      <c r="V35" s="43"/>
       <c r="W35" s="43"/>
       <c r="X35" s="43"/>
       <c r="Y35" s="43"/>
@@ -4635,87 +4690,603 @@
       <c r="BL35" s="21"/>
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20" t="str">
+      <c r="A36" s="25"/>
+      <c r="B36" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="84"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
+      <c r="S36" s="43"/>
+      <c r="T36" s="43"/>
+      <c r="U36" s="43"/>
+      <c r="V36" s="43"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="43"/>
+      <c r="Y36" s="43"/>
+      <c r="Z36" s="43"/>
+      <c r="AA36" s="43"/>
+      <c r="AB36" s="43"/>
+      <c r="AC36" s="43"/>
+      <c r="AD36" s="43"/>
+      <c r="AE36" s="43"/>
+      <c r="AF36" s="43"/>
+      <c r="AG36" s="43"/>
+      <c r="AH36" s="43"/>
+      <c r="AI36" s="43"/>
+      <c r="AJ36" s="43"/>
+      <c r="AK36" s="43"/>
+      <c r="AL36" s="43"/>
+      <c r="AM36" s="43"/>
+      <c r="AN36" s="43"/>
+      <c r="AO36" s="43"/>
+      <c r="AP36" s="43"/>
+      <c r="AQ36" s="43"/>
+      <c r="AR36" s="43"/>
+      <c r="AS36" s="43"/>
+      <c r="AT36" s="43"/>
+      <c r="AU36" s="43"/>
+      <c r="AV36" s="43"/>
+      <c r="AW36" s="43"/>
+      <c r="AX36" s="43"/>
+      <c r="AY36" s="43"/>
+      <c r="AZ36" s="43"/>
+      <c r="BA36" s="43"/>
+      <c r="BB36" s="43"/>
+      <c r="BC36" s="43"/>
+      <c r="BD36" s="43"/>
+      <c r="BE36" s="43"/>
+      <c r="BF36" s="43"/>
+      <c r="BG36" s="43"/>
+      <c r="BH36" s="43"/>
+      <c r="BI36" s="43"/>
+      <c r="BJ36" s="21"/>
+      <c r="BK36" s="21"/>
+      <c r="BL36" s="21"/>
+    </row>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
+      <c r="B37" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="81">
+        <v>1</v>
+      </c>
+      <c r="E37" s="82">
+        <v>44316</v>
+      </c>
+      <c r="F37" s="82">
+        <v>44323</v>
+      </c>
+      <c r="G37" s="60"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="43"/>
+      <c r="T37" s="43"/>
+      <c r="U37" s="43"/>
+      <c r="V37" s="43"/>
+      <c r="W37" s="43"/>
+      <c r="X37" s="43"/>
+      <c r="Y37" s="43"/>
+      <c r="Z37" s="43"/>
+      <c r="AA37" s="43"/>
+      <c r="AB37" s="43"/>
+      <c r="AC37" s="43"/>
+      <c r="AD37" s="43"/>
+      <c r="AE37" s="43"/>
+      <c r="AF37" s="43"/>
+      <c r="AG37" s="43"/>
+      <c r="AH37" s="43"/>
+      <c r="AI37" s="43"/>
+      <c r="AJ37" s="43"/>
+      <c r="AK37" s="43"/>
+      <c r="AL37" s="43"/>
+      <c r="AM37" s="43"/>
+      <c r="AN37" s="43"/>
+      <c r="AO37" s="43"/>
+      <c r="AP37" s="43"/>
+      <c r="AQ37" s="43"/>
+      <c r="AR37" s="43"/>
+      <c r="AS37" s="43"/>
+      <c r="AT37" s="43"/>
+      <c r="AU37" s="43"/>
+      <c r="AV37" s="43"/>
+      <c r="AW37" s="43"/>
+      <c r="AX37" s="43"/>
+      <c r="AY37" s="43"/>
+      <c r="AZ37" s="43"/>
+      <c r="BA37" s="43"/>
+      <c r="BB37" s="43"/>
+      <c r="BC37" s="43"/>
+      <c r="BD37" s="43"/>
+      <c r="BE37" s="43"/>
+      <c r="BF37" s="43"/>
+      <c r="BG37" s="43"/>
+      <c r="BH37" s="43"/>
+      <c r="BI37" s="43"/>
+      <c r="BJ37" s="21"/>
+      <c r="BK37" s="21"/>
+      <c r="BL37" s="21"/>
+    </row>
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="81">
+        <v>1</v>
+      </c>
+      <c r="E38" s="82">
+        <v>44316</v>
+      </c>
+      <c r="F38" s="82">
+        <v>44323</v>
+      </c>
+      <c r="G38" s="60"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="43"/>
+      <c r="T38" s="43"/>
+      <c r="U38" s="43"/>
+      <c r="V38" s="43"/>
+      <c r="W38" s="43"/>
+      <c r="X38" s="43"/>
+      <c r="Y38" s="43"/>
+      <c r="Z38" s="43"/>
+      <c r="AA38" s="43"/>
+      <c r="AB38" s="43"/>
+      <c r="AC38" s="43"/>
+      <c r="AD38" s="43"/>
+      <c r="AE38" s="43"/>
+      <c r="AF38" s="43"/>
+      <c r="AG38" s="43"/>
+      <c r="AH38" s="43"/>
+      <c r="AI38" s="43"/>
+      <c r="AJ38" s="43"/>
+      <c r="AK38" s="43"/>
+      <c r="AL38" s="43"/>
+      <c r="AM38" s="43"/>
+      <c r="AN38" s="43"/>
+      <c r="AO38" s="43"/>
+      <c r="AP38" s="43"/>
+      <c r="AQ38" s="43"/>
+      <c r="AR38" s="43"/>
+      <c r="AS38" s="43"/>
+      <c r="AT38" s="43"/>
+      <c r="AU38" s="43"/>
+      <c r="AV38" s="43"/>
+      <c r="AW38" s="43"/>
+      <c r="AX38" s="43"/>
+      <c r="AY38" s="43"/>
+      <c r="AZ38" s="43"/>
+      <c r="BA38" s="43"/>
+      <c r="BB38" s="43"/>
+      <c r="BC38" s="43"/>
+      <c r="BD38" s="43"/>
+      <c r="BE38" s="43"/>
+      <c r="BF38" s="43"/>
+      <c r="BG38" s="43"/>
+      <c r="BH38" s="43"/>
+      <c r="BI38" s="43"/>
+      <c r="BJ38" s="21"/>
+      <c r="BK38" s="21"/>
+      <c r="BL38" s="21"/>
+    </row>
+    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25"/>
+      <c r="B39" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="81">
+        <v>1</v>
+      </c>
+      <c r="E39" s="82">
+        <v>44316</v>
+      </c>
+      <c r="F39" s="82">
+        <v>44330</v>
+      </c>
+      <c r="G39" s="60"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="43"/>
+      <c r="T39" s="43"/>
+      <c r="U39" s="43"/>
+      <c r="V39" s="43"/>
+      <c r="W39" s="43"/>
+      <c r="X39" s="43"/>
+      <c r="Y39" s="43"/>
+      <c r="Z39" s="43"/>
+      <c r="AA39" s="43"/>
+      <c r="AB39" s="43"/>
+      <c r="AC39" s="43"/>
+      <c r="AD39" s="43"/>
+      <c r="AE39" s="43"/>
+      <c r="AF39" s="43"/>
+      <c r="AG39" s="43"/>
+      <c r="AH39" s="43"/>
+      <c r="AI39" s="43"/>
+      <c r="AJ39" s="43"/>
+      <c r="AK39" s="43"/>
+      <c r="AL39" s="43"/>
+      <c r="AM39" s="43"/>
+      <c r="AN39" s="43"/>
+      <c r="AO39" s="43"/>
+      <c r="AP39" s="43"/>
+      <c r="AQ39" s="43"/>
+      <c r="AR39" s="43"/>
+      <c r="AS39" s="43"/>
+      <c r="AT39" s="43"/>
+      <c r="AU39" s="43"/>
+      <c r="AV39" s="43"/>
+      <c r="AW39" s="43"/>
+      <c r="AX39" s="43"/>
+      <c r="AY39" s="43"/>
+      <c r="AZ39" s="43"/>
+      <c r="BA39" s="43"/>
+      <c r="BB39" s="43"/>
+      <c r="BC39" s="43"/>
+      <c r="BD39" s="43"/>
+      <c r="BE39" s="43"/>
+      <c r="BF39" s="43"/>
+      <c r="BG39" s="43"/>
+      <c r="BH39" s="43"/>
+      <c r="BI39" s="43"/>
+      <c r="BJ39" s="21"/>
+      <c r="BK39" s="21"/>
+      <c r="BL39" s="21"/>
+    </row>
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="25"/>
+      <c r="B40" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="81">
+        <v>1</v>
+      </c>
+      <c r="E40" s="82">
+        <v>44316</v>
+      </c>
+      <c r="F40" s="82">
+        <v>44323</v>
+      </c>
+      <c r="G40" s="60"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="43"/>
+      <c r="T40" s="43"/>
+      <c r="U40" s="43"/>
+      <c r="V40" s="43"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="43"/>
+      <c r="Y40" s="43"/>
+      <c r="Z40" s="43"/>
+      <c r="AA40" s="43"/>
+      <c r="AB40" s="43"/>
+      <c r="AC40" s="43"/>
+      <c r="AD40" s="43"/>
+      <c r="AE40" s="43"/>
+      <c r="AF40" s="43"/>
+      <c r="AG40" s="43"/>
+      <c r="AH40" s="43"/>
+      <c r="AI40" s="43"/>
+      <c r="AJ40" s="43"/>
+      <c r="AK40" s="43"/>
+      <c r="AL40" s="43"/>
+      <c r="AM40" s="43"/>
+      <c r="AN40" s="43"/>
+      <c r="AO40" s="43"/>
+      <c r="AP40" s="43"/>
+      <c r="AQ40" s="43"/>
+      <c r="AR40" s="43"/>
+      <c r="AS40" s="43"/>
+      <c r="AT40" s="43"/>
+      <c r="AU40" s="43"/>
+      <c r="AV40" s="43"/>
+      <c r="AW40" s="43"/>
+      <c r="AX40" s="43"/>
+      <c r="AY40" s="43"/>
+      <c r="AZ40" s="43"/>
+      <c r="BA40" s="43"/>
+      <c r="BB40" s="43"/>
+      <c r="BC40" s="43"/>
+      <c r="BD40" s="43"/>
+      <c r="BE40" s="43"/>
+      <c r="BF40" s="43"/>
+      <c r="BG40" s="43"/>
+      <c r="BH40" s="43"/>
+      <c r="BI40" s="43"/>
+      <c r="BJ40" s="21"/>
+      <c r="BK40" s="21"/>
+      <c r="BL40" s="21"/>
+    </row>
+    <row r="41" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25"/>
+      <c r="B41" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="75"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="43"/>
+      <c r="T41" s="43"/>
+      <c r="U41" s="43"/>
+      <c r="V41" s="43"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="43"/>
+      <c r="Y41" s="43"/>
+      <c r="Z41" s="43"/>
+      <c r="AA41" s="43"/>
+      <c r="AB41" s="43"/>
+      <c r="AC41" s="43"/>
+      <c r="AD41" s="43"/>
+      <c r="AE41" s="43"/>
+      <c r="AF41" s="43"/>
+      <c r="AG41" s="43"/>
+      <c r="AH41" s="43"/>
+      <c r="AI41" s="43"/>
+      <c r="AJ41" s="43"/>
+      <c r="AK41" s="43"/>
+      <c r="AL41" s="43"/>
+      <c r="AM41" s="43"/>
+      <c r="AN41" s="43"/>
+      <c r="AO41" s="43"/>
+      <c r="AP41" s="43"/>
+      <c r="AQ41" s="43"/>
+      <c r="AR41" s="43"/>
+      <c r="AS41" s="43"/>
+      <c r="AT41" s="43"/>
+      <c r="AU41" s="43"/>
+      <c r="AV41" s="43"/>
+      <c r="AW41" s="43"/>
+      <c r="AX41" s="43"/>
+      <c r="AY41" s="43"/>
+      <c r="AZ41" s="43"/>
+      <c r="BA41" s="43"/>
+      <c r="BB41" s="43"/>
+      <c r="BC41" s="43"/>
+      <c r="BD41" s="43"/>
+      <c r="BE41" s="43"/>
+      <c r="BF41" s="43"/>
+      <c r="BG41" s="43"/>
+      <c r="BH41" s="43"/>
+      <c r="BI41" s="43"/>
+      <c r="BJ41" s="21"/>
+      <c r="BK41" s="21"/>
+      <c r="BL41" s="21"/>
+    </row>
+    <row r="42" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="78">
+        <v>1</v>
+      </c>
+      <c r="E42" s="73">
+        <v>44323</v>
+      </c>
+      <c r="F42" s="73">
+        <v>44330</v>
+      </c>
+      <c r="G42" s="60"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="43"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
+      <c r="Y42" s="43"/>
+      <c r="Z42" s="43"/>
+      <c r="AA42" s="43"/>
+      <c r="AB42" s="43"/>
+      <c r="AC42" s="43"/>
+      <c r="AD42" s="43"/>
+      <c r="AE42" s="43"/>
+      <c r="AF42" s="43"/>
+      <c r="AG42" s="43"/>
+      <c r="AH42" s="43"/>
+      <c r="AI42" s="43"/>
+      <c r="AJ42" s="43"/>
+      <c r="AK42" s="43"/>
+      <c r="AL42" s="43"/>
+      <c r="AM42" s="43"/>
+      <c r="AN42" s="43"/>
+      <c r="AO42" s="43"/>
+      <c r="AP42" s="43"/>
+      <c r="AQ42" s="43"/>
+      <c r="AR42" s="43"/>
+      <c r="AS42" s="43"/>
+      <c r="AT42" s="43"/>
+      <c r="AU42" s="43"/>
+      <c r="AV42" s="43"/>
+      <c r="AW42" s="43"/>
+      <c r="AX42" s="43"/>
+      <c r="AY42" s="43"/>
+      <c r="AZ42" s="43"/>
+      <c r="BA42" s="43"/>
+      <c r="BB42" s="43"/>
+      <c r="BC42" s="43"/>
+      <c r="BD42" s="43"/>
+      <c r="BE42" s="43"/>
+      <c r="BF42" s="43"/>
+      <c r="BG42" s="43"/>
+      <c r="BH42" s="43"/>
+      <c r="BI42" s="43"/>
+      <c r="BJ42" s="21"/>
+      <c r="BK42" s="21"/>
+      <c r="BL42" s="21"/>
+    </row>
+    <row r="43" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
-      <c r="U36" s="22"/>
-      <c r="V36" s="22"/>
-      <c r="W36" s="22"/>
-      <c r="X36" s="22"/>
-      <c r="Y36" s="22"/>
-      <c r="Z36" s="22"/>
-      <c r="AA36" s="22"/>
-      <c r="AB36" s="22"/>
-      <c r="AC36" s="22"/>
-      <c r="AD36" s="22"/>
-      <c r="AE36" s="22"/>
-      <c r="AF36" s="22"/>
-      <c r="AG36" s="22"/>
-      <c r="AH36" s="22"/>
-      <c r="AI36" s="22"/>
-      <c r="AJ36" s="22"/>
-      <c r="AK36" s="22"/>
-      <c r="AL36" s="22"/>
-      <c r="AM36" s="22"/>
-      <c r="AN36" s="22"/>
-      <c r="AO36" s="22"/>
-      <c r="AP36" s="22"/>
-      <c r="AQ36" s="22"/>
-      <c r="AR36" s="22"/>
-      <c r="AS36" s="22"/>
-      <c r="AT36" s="22"/>
-      <c r="AU36" s="22"/>
-      <c r="AV36" s="22"/>
-      <c r="AW36" s="22"/>
-      <c r="AX36" s="22"/>
-      <c r="AY36" s="22"/>
-      <c r="AZ36" s="22"/>
-      <c r="BA36" s="22"/>
-      <c r="BB36" s="22"/>
-      <c r="BC36" s="22"/>
-      <c r="BD36" s="22"/>
-      <c r="BE36" s="22"/>
-      <c r="BF36" s="22"/>
-      <c r="BG36" s="22"/>
-      <c r="BH36" s="22"/>
-      <c r="BI36" s="22"/>
-      <c r="BJ36" s="22"/>
-      <c r="BK36" s="22"/>
-      <c r="BL36" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
+      <c r="Z43" s="22"/>
+      <c r="AA43" s="22"/>
+      <c r="AB43" s="22"/>
+      <c r="AC43" s="22"/>
+      <c r="AD43" s="22"/>
+      <c r="AE43" s="22"/>
+      <c r="AF43" s="22"/>
+      <c r="AG43" s="22"/>
+      <c r="AH43" s="22"/>
+      <c r="AI43" s="22"/>
+      <c r="AJ43" s="22"/>
+      <c r="AK43" s="22"/>
+      <c r="AL43" s="22"/>
+      <c r="AM43" s="22"/>
+      <c r="AN43" s="22"/>
+      <c r="AO43" s="22"/>
+      <c r="AP43" s="22"/>
+      <c r="AQ43" s="22"/>
+      <c r="AR43" s="22"/>
+      <c r="AS43" s="22"/>
+      <c r="AT43" s="22"/>
+      <c r="AU43" s="22"/>
+      <c r="AV43" s="22"/>
+      <c r="AW43" s="22"/>
+      <c r="AX43" s="22"/>
+      <c r="AY43" s="22"/>
+      <c r="AZ43" s="22"/>
+      <c r="BA43" s="22"/>
+      <c r="BB43" s="22"/>
+      <c r="BC43" s="22"/>
+      <c r="BD43" s="22"/>
+      <c r="BE43" s="22"/>
+      <c r="BF43" s="22"/>
+      <c r="BG43" s="22"/>
+      <c r="BH43" s="22"/>
+      <c r="BI43" s="22"/>
+      <c r="BJ43" s="22"/>
+      <c r="BK43" s="22"/>
+      <c r="BL43" s="22"/>
     </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G37" s="6"/>
+    <row r="44" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="6"/>
     </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="11"/>
-      <c r="F38" s="26"/>
+    <row r="45" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="11"/>
+      <c r="F45" s="26"/>
     </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="12"/>
+    <row r="46" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4730,8 +5301,8 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D9 D36 D11 D19 D24">
-    <cfRule type="dataBar" priority="84">
+  <conditionalFormatting sqref="D7:D9 D43 D11 D19 D24 D37:D40">
+    <cfRule type="dataBar" priority="86">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4744,21 +5315,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL36">
-    <cfRule type="expression" dxfId="2" priority="103">
+  <conditionalFormatting sqref="I5:BL43">
+    <cfRule type="expression" dxfId="2" priority="105">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="1" priority="97">
+  <conditionalFormatting sqref="I7:BL43">
+    <cfRule type="expression" dxfId="1" priority="99">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="100" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="dataBar" priority="65">
+    <cfRule type="dataBar" priority="67">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4772,7 +5343,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4786,7 +5357,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="dataBar" priority="58">
+    <cfRule type="dataBar" priority="60">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4800,7 +5371,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16 D18">
-    <cfRule type="dataBar" priority="62">
+    <cfRule type="dataBar" priority="64">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4814,7 +5385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D18">
-    <cfRule type="dataBar" priority="61">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4828,7 +5399,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="dataBar" priority="60">
+    <cfRule type="dataBar" priority="62">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4842,7 +5413,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14">
-    <cfRule type="dataBar" priority="57">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4856,7 +5427,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="dataBar" priority="54">
+    <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4870,7 +5441,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4884,7 +5455,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="dataBar" priority="52">
+    <cfRule type="dataBar" priority="54">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4898,7 +5469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="dataBar" priority="51">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4912,7 +5483,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="dataBar" priority="50">
+    <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4926,7 +5497,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4940,7 +5511,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="dataBar" priority="48">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4954,7 +5525,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22">
-    <cfRule type="dataBar" priority="47">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4968,7 +5539,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="dataBar" priority="44">
+    <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4982,7 +5553,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="dataBar" priority="43">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4996,7 +5567,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5010,7 +5581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="43">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5024,7 +5595,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="dataBar" priority="40">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5038,7 +5609,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5052,7 +5623,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="dataBar" priority="32">
+    <cfRule type="dataBar" priority="34">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5066,7 +5637,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5080,7 +5651,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="dataBar" priority="36">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5094,7 +5665,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5108,7 +5679,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="dataBar" priority="30">
+    <cfRule type="dataBar" priority="32">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5122,7 +5693,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5136,7 +5707,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5150,7 +5721,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5164,7 +5735,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D31">
-    <cfRule type="dataBar" priority="28">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5178,7 +5749,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D31">
-    <cfRule type="dataBar" priority="27">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5192,7 +5763,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5206,7 +5777,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5219,8 +5790,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5233,8 +5804,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5248,7 +5819,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5262,7 +5833,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5276,7 +5847,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5289,8 +5860,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="11">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5303,8 +5874,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="10">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5317,8 +5888,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5331,8 +5902,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="16">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5345,8 +5916,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="15">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5359,8 +5930,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="12">
+  <conditionalFormatting sqref="D35 D42">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5373,8 +5944,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5387,8 +5958,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5401,8 +5972,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5415,8 +5986,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5429,8 +6000,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5443,8 +6014,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5457,8 +6028,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5471,8 +6042,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="D34:D35 D42">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5481,6 +6052,34 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{AB54FE81-C321-4B4A-B6E0-6742B469016C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7B79EC1A-5F64-41DA-BBA1-3CE03E7D8310}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A6319B33-55A5-4CCB-98B8-A9FDAB51FEF6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5512,7 +6111,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D9 D36 D11 D19 D24</xm:sqref>
+          <xm:sqref>D7:D9 D43 D11 D19 D24 D37:D40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6A02471B-CBED-420D-A71B-22E39791D61B}">
@@ -6022,7 +6621,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0BC38917-7F43-4FDA-9C25-B487537A13AA}">
@@ -6037,7 +6636,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C259914D-3D04-4DEE-81A6-2E8DE5BFDFBC}">
@@ -6097,7 +6696,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AE0DBD5C-8468-4D5A-B9F3-401B50C12A1E}">
@@ -6112,7 +6711,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{12DD82C2-8CF8-44E6-B4A6-986E3DFCAA5B}">
@@ -6127,7 +6726,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1E2CA01B-C885-4B1B-BDAC-867236E441C3}">
@@ -6142,7 +6741,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1723A971-90BD-4903-AE9E-378A023BABFE}">
@@ -6157,7 +6756,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4082F14F-772E-4E73-88DD-ECDF3475480F}">
@@ -6172,7 +6771,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1712A78B-5806-460E-8F16-343646BF490C}">
@@ -6187,7 +6786,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{18DAFC6D-9391-4FFD-9844-A9606E70A44F}">
@@ -6202,7 +6801,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{83CC43A2-3757-497C-AE47-023D422DE77D}">
@@ -6217,7 +6816,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{474B52C7-F05E-484C-AE4A-7B839432ECC5}">
@@ -6232,7 +6831,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{13FBE554-EF1C-4F9F-9C79-CDA8BF51BB3C}">
@@ -6247,7 +6846,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F6262373-9022-4846-A0A7-0503744D09E2}">
@@ -6262,7 +6861,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{25BF47B7-FDB3-45FE-905A-B91AC0BA472D}">
@@ -6277,7 +6876,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AB54FE81-C321-4B4A-B6E0-6742B469016C}">
@@ -6292,7 +6891,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D34:D35 D42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7B79EC1A-5F64-41DA-BBA1-3CE03E7D8310}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D36</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A6319B33-55A5-4CCB-98B8-A9FDAB51FEF6}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>